<commit_message>
Session 3 update with self-report pre-treatment phase measurements
</commit_message>
<xml_diff>
--- a/data/GASY_brief_self.xlsx
+++ b/data/GASY_brief_self.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/participant_2_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26D5C36-2A47-C147-9583-08FB9451566D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30359B0A-E3BB-F94D-85E5-BDEC58D38301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="600" windowWidth="27640" windowHeight="15800" xr2:uid="{8AD1997E-D8CB-5944-A1E2-519BC3D1F2A2}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,10 +438,10 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
@@ -449,7 +449,7 @@
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,102 +463,135 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="C2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="C3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="C4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="C7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="C9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="C10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>76</v>
+      </c>
+      <c r="C14">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final outcome measures added
</commit_message>
<xml_diff>
--- a/data/GASY_brief_self.xlsx
+++ b/data/GASY_brief_self.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GASY/participant_2_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9502139-94F2-6344-8D82-A2304BABF3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0783ED-FD88-B747-AB79-C20A2102DBA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="840" windowWidth="27640" windowHeight="15800" xr2:uid="{8AD1997E-D8CB-5944-A1E2-519BC3D1F2A2}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,6 +467,9 @@
       <c r="C2">
         <v>55</v>
       </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -478,6 +481,9 @@
       <c r="C3">
         <v>51</v>
       </c>
+      <c r="D3">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -489,6 +495,9 @@
       <c r="C4">
         <v>53</v>
       </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -500,6 +509,9 @@
       <c r="C5">
         <v>71</v>
       </c>
+      <c r="D5">
+        <v>64</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -511,6 +523,9 @@
       <c r="C6">
         <v>75</v>
       </c>
+      <c r="D6">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -522,6 +537,9 @@
       <c r="C7">
         <v>75</v>
       </c>
+      <c r="D7">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -533,6 +551,9 @@
       <c r="C8">
         <v>82</v>
       </c>
+      <c r="D8">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -544,6 +565,9 @@
       <c r="C9">
         <v>78</v>
       </c>
+      <c r="D9">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -555,6 +579,9 @@
       <c r="C10">
         <v>63</v>
       </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -566,6 +593,9 @@
       <c r="C11">
         <v>75</v>
       </c>
+      <c r="D11">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -576,6 +606,9 @@
       </c>
       <c r="C12">
         <v>71</v>
+      </c>
+      <c r="D12">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>